<commit_message>
add start/resume on env and fix pagerank db
</commit_message>
<xml_diff>
--- a/docs/api testing.xlsx
+++ b/docs/api testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazua\Documents\search-engine\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CFE8B5-CDBD-4EB3-A60E-5D541148CC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F212617E-A46A-469C-96D6-F91FFD3FD7C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{53B28172-300E-444A-8214-462D2500A65B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Route</t>
   </si>
@@ -117,6 +117,21 @@
   </si>
   <si>
     <t>76 ms</t>
+  </si>
+  <si>
+    <t>581 ms</t>
+  </si>
+  <si>
+    <t>796 ms</t>
+  </si>
+  <si>
+    <t>1826 ms</t>
+  </si>
+  <si>
+    <t>Rata-rata Response Time</t>
+  </si>
+  <si>
+    <t>Jumlah Request</t>
   </si>
 </sst>
 </file>
@@ -204,9 +219,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -217,6 +229,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -533,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D4CC9D3-9377-477A-A3AC-226BEAD2D173}">
-  <dimension ref="G7:I16"/>
+  <dimension ref="G7:M16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,111 +559,137 @@
     <col min="7" max="7" width="37.28515625" customWidth="1"/>
     <col min="8" max="8" width="40.42578125" customWidth="1"/>
     <col min="9" max="9" width="34.5703125" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="13" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="7:9" x14ac:dyDescent="0.25">
-      <c r="G7" s="2" t="s">
+    <row r="7" spans="7:13" x14ac:dyDescent="0.25">
+      <c r="G7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="7:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="G8" s="2"/>
-      <c r="H8" s="5" t="s">
+      <c r="I7" s="5"/>
+      <c r="L7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="7:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G8" s="6"/>
+      <c r="H8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="7:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L8" s="2">
+        <v>100</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="7:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I9" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="10" spans="7:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L9" s="2">
+        <v>1000</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="7:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="I10" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="7:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="L10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="7:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="7:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="7:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="G12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="7:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="7:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="G13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="I13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="7:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="7:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="G14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="7:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="7:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="G15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="7:9" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="7:13" ht="31.5" x14ac:dyDescent="0.25">
       <c r="G16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="I16" s="2" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>